<commit_message>
uploads: update all templates to not have columns selected, and to have either number (5 decimal) or text formats only (removed "general" format)
</commit_message>
<xml_diff>
--- a/database/files/prof/business-upload/department_upload_template.xlsx
+++ b/database/files/prof/business-upload/department_upload_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dakahle\work\fin-dfa\database\files\business-upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dakahle\work\fin-dfa\database\files\prof\business-upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -207,15 +207,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -234,6 +227,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,49 +545,49 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.1796875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="55.81640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="10"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -606,50 +607,50 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40" style="7" customWidth="1"/>
-    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="1" max="1" width="40" style="4" customWidth="1"/>
+    <col min="2" max="2" width="38" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10"/>
-    </row>
-    <row r="2" spans="1:2" ht="50" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
     </row>
@@ -659,7 +660,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>